<commit_message>
nueva api y nueva interfaz consultas sq
</commit_message>
<xml_diff>
--- a/Plantilla importar_ventas/importar ventas.xlsx
+++ b/Plantilla importar_ventas/importar ventas.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ricardo\Documents\predictive_software\Plantilla importar_ventas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{824C85B1-2383-4749-B0F1-3E85DC32B30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A0EEEC-6B55-41F3-ABE5-E863C3845A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{04F80AFC-6EF6-4EB5-904F-1BD31C458112}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{04F80AFC-6EF6-4EB5-904F-1BD31C458112}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>COD_VENTA</t>
   </si>
@@ -53,26 +56,41 @@
     <t>ANIO</t>
   </si>
   <si>
-    <t>TOTAL_PROD_VENDIDOS</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
-    <t>G-65651111</t>
-  </si>
-  <si>
-    <t>2023-06</t>
+    <t>PRODUCTO</t>
+  </si>
+  <si>
+    <t>Semirremolques</t>
+  </si>
+  <si>
+    <t>Remolques</t>
+  </si>
+  <si>
+    <t>G-65651118</t>
+  </si>
+  <si>
+    <t>G-65651119</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,8 +116,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1496A880-1756-48CD-90BF-BE457D316E84}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,8 +449,8 @@
     <col min="3" max="3" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -455,26 +477,55 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+      <c r="D2">
         <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>23</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
       </c>
       <c r="E2">
         <v>2023</v>
       </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2" si="0">E2&amp;"-"&amp;D2</f>
+        <v>2023-7</v>
+      </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>2023</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3" si="1">E3&amp;"-"&amp;D3</f>
+        <v>2023-7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>